<commit_message>
2016 benchmarks: C++ // Java 8 // NodeJS // PHP 7.0 // Python 3.5 // Python 2.7 // Perl 5 // PHP 5.6
</commit_message>
<xml_diff>
--- a/results/data.xlsx
+++ b/results/data.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="54" windowWidth="18503" windowHeight="7023" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="54" windowWidth="18503" windowHeight="7023"/>
   </bookViews>
   <sheets>
-    <sheet name="2012" sheetId="1" r:id="rId1"/>
-    <sheet name="redo-2016" sheetId="2" r:id="rId2"/>
+    <sheet name="2016" sheetId="3" r:id="rId1"/>
+    <sheet name="~2013" sheetId="2" r:id="rId2"/>
+    <sheet name="2010" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="55">
   <si>
     <t>Language</t>
   </si>
@@ -133,6 +134,54 @@
   </si>
   <si>
     <t>(OpenJDK)</t>
+  </si>
+  <si>
+    <t>g++ 5.3.1</t>
+  </si>
+  <si>
+    <t>1.8.0_72</t>
+  </si>
+  <si>
+    <t>Java 8 (non-std lib)</t>
+  </si>
+  <si>
+    <t>PHP 7.0</t>
+  </si>
+  <si>
+    <t>7.0.2</t>
+  </si>
+  <si>
+    <t>4.2.6</t>
+  </si>
+  <si>
+    <t>Java 8</t>
+  </si>
+  <si>
+    <t>Python 3.5</t>
+  </si>
+  <si>
+    <t>3.5.1</t>
+  </si>
+  <si>
+    <t>2.7.11</t>
+  </si>
+  <si>
+    <t>5.22.1</t>
+  </si>
+  <si>
+    <t>PHP 5.6</t>
+  </si>
+  <si>
+    <t>5.6.17</t>
+  </si>
+  <si>
+    <t>(NTS)</t>
+  </si>
+  <si>
+    <t>32-bit system</t>
+  </si>
+  <si>
+    <t>64-bit system</t>
   </si>
 </sst>
 </file>
@@ -142,7 +191,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,6 +212,13 @@
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -189,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -211,16 +267,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -524,68 +597,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="10" t="s">
+      <c r="F1" s="13"/>
+      <c r="G1" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="14"/>
+      <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="9"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="G2" s="14"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="3">
-        <v>1.52</v>
+        <v>0.95199999999999996</v>
       </c>
       <c r="C3" s="3">
-        <v>0.188</v>
+        <v>0.17199999999999999</v>
       </c>
       <c r="D3" s="3">
         <f>B3+C3</f>
-        <v>1.708</v>
+        <v>1.1239999999999999</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>18</v>
@@ -594,221 +666,261 @@
         <v>18</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="12">
-        <v>2.4460000000000002</v>
-      </c>
-      <c r="C4" s="12">
-        <v>0.15</v>
-      </c>
-      <c r="D4" s="12">
-        <f t="shared" ref="D4:D11" si="0">B4+C4</f>
-        <v>2.5960000000000001</v>
-      </c>
-      <c r="E4" s="13">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="10">
+        <v>1.3320000000000001</v>
+      </c>
+      <c r="C4" s="10">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="D4" s="10">
+        <f t="shared" ref="D4:D12" si="0">B4+C4</f>
+        <v>1.4280000000000002</v>
+      </c>
+      <c r="E4" s="11">
         <f>(D4-$D$3)/$D$3</f>
-        <v>0.51990632318501184</v>
-      </c>
-      <c r="F4" s="13">
+        <v>0.27046263345195753</v>
+      </c>
+      <c r="F4" s="11">
         <f>E4</f>
-        <v>0.51990632318501184</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+        <v>0.27046263345195753</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="16">
+        <v>1.524</v>
+      </c>
+      <c r="C5" s="16">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="D5" s="16">
+        <f t="shared" si="0"/>
+        <v>2.04</v>
+      </c>
+      <c r="E5" s="17">
+        <f>(D5-$D$3)/$D$3</f>
+        <v>0.81494661921708211</v>
+      </c>
+      <c r="F5" s="17">
+        <f t="shared" ref="F5:F12" si="1">(D5-D4)/D4</f>
+        <v>0.42857142857142844</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="12">
-        <v>3.2080000000000002</v>
-      </c>
-      <c r="C5" s="12">
+      <c r="B6" s="10">
+        <v>2.988</v>
+      </c>
+      <c r="C6" s="10">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="D6" s="10">
+        <f>B6+C6</f>
+        <v>3.1560000000000001</v>
+      </c>
+      <c r="E6" s="11">
+        <f t="shared" ref="E6:E12" si="2">(D6-$D$3)/$D$3</f>
+        <v>1.8078291814946621</v>
+      </c>
+      <c r="F6" s="11">
+        <f t="shared" si="1"/>
+        <v>0.54705882352941182</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="16">
+        <v>6.524</v>
+      </c>
+      <c r="C7" s="16">
         <v>0.184</v>
       </c>
-      <c r="D5" s="12">
-        <f t="shared" si="0"/>
-        <v>3.3920000000000003</v>
-      </c>
-      <c r="E5" s="13">
-        <f>(D5-$D$3)/$D$3</f>
-        <v>0.98594847775175665</v>
-      </c>
-      <c r="F5" s="13">
-        <f t="shared" ref="F5:F11" si="1">(D5-D4)/D4</f>
-        <v>0.3066255778120186</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="3">
-        <v>4.0679999999999996</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0.54400000000000004</v>
-      </c>
-      <c r="D6" s="3">
-        <f>B6+C6</f>
-        <v>4.6120000000000001</v>
-      </c>
-      <c r="E6" s="4">
-        <f t="shared" ref="E6:E11" si="2">(D6-$D$3)/$D$3</f>
-        <v>1.7002341920374706</v>
-      </c>
-      <c r="F6" s="4">
-        <f t="shared" si="1"/>
-        <v>0.3596698113207546</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="3">
-        <v>8.5210000000000008</v>
-      </c>
-      <c r="C7" s="3">
-        <v>0.192</v>
-      </c>
-      <c r="D7" s="3">
+      <c r="D7" s="16">
         <f>B7+C7</f>
-        <v>8.713000000000001</v>
-      </c>
-      <c r="E7" s="4">
-        <f t="shared" si="2"/>
-        <v>4.1012880562060898</v>
-      </c>
-      <c r="F7" s="4">
-        <f t="shared" si="1"/>
-        <v>0.88920208152645286</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>29</v>
+        <v>6.7080000000000002</v>
+      </c>
+      <c r="E7" s="17">
+        <f t="shared" ref="E7" si="3">(D7-$D$3)/$D$3</f>
+        <v>4.9679715302491116</v>
+      </c>
+      <c r="F7" s="17">
+        <f>(D7-D5)/D5</f>
+        <v>2.2882352941176469</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>45</v>
       </c>
       <c r="B8" s="3">
-        <v>13.305</v>
+        <v>14.616</v>
       </c>
       <c r="C8" s="3">
-        <v>0.152</v>
+        <v>0.90800000000000003</v>
       </c>
       <c r="D8" s="3">
-        <f t="shared" si="0"/>
-        <v>13.456999999999999</v>
+        <f>B8+C8</f>
+        <v>15.523999999999999</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="2"/>
-        <v>6.8788056206088983</v>
+        <v>12.811387900355871</v>
       </c>
       <c r="F8" s="4">
-        <f t="shared" si="1"/>
-        <v>0.54447377481923531</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+        <f>(D8-D6)/D6</f>
+        <v>3.9188846641318116</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="3">
+        <v>18.655999999999999</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="D9" s="3">
+        <f>B9+C9</f>
+        <v>19.003999999999998</v>
+      </c>
+      <c r="E9" s="4">
+        <f>(D9-$D$3)/$D$3</f>
+        <v>15.907473309608541</v>
+      </c>
+      <c r="F9" s="4">
+        <f>(D9-D8)/D8</f>
+        <v>0.22416902860087598</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="3">
-        <v>27.885999999999999</v>
-      </c>
-      <c r="C9" s="3">
-        <v>0.16800000000000001</v>
-      </c>
-      <c r="D9" s="3">
-        <f t="shared" si="0"/>
-        <v>28.053999999999998</v>
-      </c>
-      <c r="E9" s="4">
-        <f t="shared" si="2"/>
-        <v>15.425058548009368</v>
-      </c>
-      <c r="F9" s="4">
-        <f t="shared" si="1"/>
-        <v>1.0847142750984617</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B10" s="3">
+        <v>20.776</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="D10" s="3">
+        <f>B10+C10</f>
+        <v>21.111999999999998</v>
+      </c>
+      <c r="E10" s="4">
+        <f>(D10-$D$3)/$D$3</f>
+        <v>17.782918149466195</v>
+      </c>
+      <c r="F10" s="4">
+        <f>(D10-D9)/D9</f>
+        <v>0.11092401599663233</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="3">
-        <v>41.670999999999999</v>
-      </c>
-      <c r="C10" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="D10" s="3">
-        <f t="shared" si="0"/>
-        <v>41.771000000000001</v>
-      </c>
-      <c r="E10" s="4">
-        <f t="shared" si="2"/>
-        <v>23.456088992974241</v>
-      </c>
-      <c r="F10" s="4">
-        <f t="shared" si="1"/>
-        <v>0.48894988236971565</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>30</v>
-      </c>
       <c r="B11" s="3">
-        <v>94.622</v>
+        <v>25.044</v>
       </c>
       <c r="C11" s="3">
-        <v>0.36399999999999999</v>
+        <v>0.23599999999999999</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" si="0"/>
-        <v>94.986000000000004</v>
+        <v>25.28</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="2"/>
-        <v>54.612412177985952</v>
+        <v>21.491103202846979</v>
       </c>
       <c r="F11" s="4">
+        <f>(D11-D10)/D10</f>
+        <v>0.19742326638878377</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="3">
+        <v>66.444000000000003</v>
+      </c>
+      <c r="C12" s="3">
+        <v>2.34</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="0"/>
+        <v>68.784000000000006</v>
+      </c>
+      <c r="E12" s="4">
+        <f t="shared" si="2"/>
+        <v>60.19572953736656</v>
+      </c>
+      <c r="F12" s="4">
         <f t="shared" si="1"/>
-        <v>1.273969979172153</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>16</v>
+        <v>1.7208860759493672</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="21" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
+    <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:D1"/>
-    <mergeCell ref="A1:A2"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:G2"/>
   </mergeCells>
@@ -821,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -831,24 +943,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="10" t="s">
+      <c r="F1" s="13"/>
+      <c r="G1" s="15" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
+      <c r="A2" s="14"/>
       <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
@@ -864,7 +976,7 @@
       <c r="F2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="9"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -891,28 +1003,28 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="10">
         <v>1.4039999999999999</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="10">
         <v>0.112</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="10">
         <f t="shared" ref="D4:D11" si="0">B4+C4</f>
         <v>1.516</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="11">
         <f>(D4-$D$3)/$D$3</f>
         <v>0.19182389937106917</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="11">
         <f>E4</f>
         <v>0.19182389937106917</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="12" t="s">
         <v>31</v>
       </c>
       <c r="H4" t="s">
@@ -920,28 +1032,28 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="10">
         <v>2.6160000000000001</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="10">
         <v>0.26800000000000002</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="10">
         <f t="shared" si="0"/>
         <v>2.8840000000000003</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="11">
         <f>(D5-$D$3)/$D$3</f>
         <v>1.267295597484277</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="11">
         <f t="shared" ref="F5:F11" si="1">(D5-D4)/D4</f>
         <v>0.90237467018469675</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="12" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1108,6 +1220,9 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="21" t="s">
+        <v>53</v>
+      </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="G13" s="6"/>
@@ -1121,4 +1236,304 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="13"/>
+      <c r="G1" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="14"/>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="14"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1.52</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.188</v>
+      </c>
+      <c r="D3" s="3">
+        <f>B3+C3</f>
+        <v>1.708</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="10">
+        <v>2.4460000000000002</v>
+      </c>
+      <c r="C4" s="10">
+        <v>0.15</v>
+      </c>
+      <c r="D4" s="10">
+        <f t="shared" ref="D4:D11" si="0">B4+C4</f>
+        <v>2.5960000000000001</v>
+      </c>
+      <c r="E4" s="11">
+        <f>(D4-$D$3)/$D$3</f>
+        <v>0.51990632318501184</v>
+      </c>
+      <c r="F4" s="11">
+        <f>E4</f>
+        <v>0.51990632318501184</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="10">
+        <v>3.2080000000000002</v>
+      </c>
+      <c r="C5" s="10">
+        <v>0.184</v>
+      </c>
+      <c r="D5" s="10">
+        <f t="shared" si="0"/>
+        <v>3.3920000000000003</v>
+      </c>
+      <c r="E5" s="11">
+        <f>(D5-$D$3)/$D$3</f>
+        <v>0.98594847775175665</v>
+      </c>
+      <c r="F5" s="11">
+        <f t="shared" ref="F5:F11" si="1">(D5-D4)/D4</f>
+        <v>0.3066255778120186</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="3">
+        <v>4.0679999999999996</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="D6" s="3">
+        <f>B6+C6</f>
+        <v>4.6120000000000001</v>
+      </c>
+      <c r="E6" s="4">
+        <f t="shared" ref="E6:E11" si="2">(D6-$D$3)/$D$3</f>
+        <v>1.7002341920374706</v>
+      </c>
+      <c r="F6" s="4">
+        <f t="shared" si="1"/>
+        <v>0.3596698113207546</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="3">
+        <v>8.5210000000000008</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.192</v>
+      </c>
+      <c r="D7" s="3">
+        <f>B7+C7</f>
+        <v>8.713000000000001</v>
+      </c>
+      <c r="E7" s="4">
+        <f t="shared" si="2"/>
+        <v>4.1012880562060898</v>
+      </c>
+      <c r="F7" s="4">
+        <f t="shared" si="1"/>
+        <v>0.88920208152645286</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="10">
+        <v>13.305</v>
+      </c>
+      <c r="C8" s="10">
+        <v>0.152</v>
+      </c>
+      <c r="D8" s="10">
+        <f t="shared" si="0"/>
+        <v>13.456999999999999</v>
+      </c>
+      <c r="E8" s="11">
+        <f t="shared" si="2"/>
+        <v>6.8788056206088983</v>
+      </c>
+      <c r="F8" s="11">
+        <f t="shared" si="1"/>
+        <v>0.54447377481923531</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="3">
+        <v>27.885999999999999</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="0"/>
+        <v>28.053999999999998</v>
+      </c>
+      <c r="E9" s="4">
+        <f t="shared" si="2"/>
+        <v>15.425058548009368</v>
+      </c>
+      <c r="F9" s="4">
+        <f t="shared" si="1"/>
+        <v>1.0847142750984617</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="3">
+        <v>41.670999999999999</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="0"/>
+        <v>41.771000000000001</v>
+      </c>
+      <c r="E10" s="4">
+        <f t="shared" si="2"/>
+        <v>23.456088992974241</v>
+      </c>
+      <c r="F10" s="4">
+        <f t="shared" si="1"/>
+        <v>0.48894988236971565</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="3">
+        <v>94.622</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="0"/>
+        <v>94.986000000000004</v>
+      </c>
+      <c r="E11" s="4">
+        <f t="shared" si="2"/>
+        <v>54.612412177985952</v>
+      </c>
+      <c r="F11" s="4">
+        <f t="shared" si="1"/>
+        <v>1.273969979172153</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Python 2.7 + PyPy
</commit_message>
<xml_diff>
--- a/results/data.xlsx
+++ b/results/data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="57">
   <si>
     <t>Language</t>
   </si>
@@ -182,6 +182,12 @@
   </si>
   <si>
     <t>64-bit system</t>
+  </si>
+  <si>
+    <t>Python 2.7 + PyPy</t>
+  </si>
+  <si>
+    <t>PyPy 4.0.1</t>
   </si>
 </sst>
 </file>
@@ -273,15 +279,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -295,6 +292,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -597,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -610,24 +616,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13" t="s">
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="15" t="s">
+      <c r="F1" s="22"/>
+      <c r="G1" s="23" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
+      <c r="A2" s="21"/>
       <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
@@ -643,10 +649,10 @@
       <c r="F2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="21"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="19" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="3">
@@ -680,7 +686,7 @@
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="D4" s="10">
-        <f t="shared" ref="D4:D12" si="0">B4+C4</f>
+        <f t="shared" ref="D4:D13" si="0">B4+C4</f>
         <v>1.4280000000000002</v>
       </c>
       <c r="E4" s="11">
@@ -699,221 +705,247 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="10">
+        <v>1.56</v>
+      </c>
+      <c r="C5" s="10">
+        <v>0.16</v>
+      </c>
+      <c r="D5" s="10">
+        <f t="shared" si="0"/>
+        <v>1.72</v>
+      </c>
+      <c r="E5" s="11">
+        <f t="shared" ref="E5:E13" si="1">(D5-$D$3)/$D$3</f>
+        <v>0.53024911032028488</v>
+      </c>
+      <c r="F5" s="11">
+        <f>(D5-D4)/D4</f>
+        <v>0.20448179271708669</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B6" s="13">
         <v>1.524</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C6" s="13">
         <v>0.51600000000000001</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D6" s="13">
         <f t="shared" si="0"/>
         <v>2.04</v>
       </c>
-      <c r="E5" s="17">
-        <f>(D5-$D$3)/$D$3</f>
+      <c r="E6" s="14">
+        <f t="shared" si="1"/>
         <v>0.81494661921708211</v>
       </c>
-      <c r="F5" s="17">
-        <f t="shared" ref="F5:F12" si="1">(D5-D4)/D4</f>
-        <v>0.42857142857142844</v>
-      </c>
-      <c r="G5" s="20" t="s">
+      <c r="F6" s="14">
+        <f t="shared" ref="F6:F13" si="2">(D6-D5)/D5</f>
+        <v>0.186046511627907</v>
+      </c>
+      <c r="G6" s="17" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B7" s="10">
         <v>2.988</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C7" s="10">
         <v>0.16800000000000001</v>
       </c>
-      <c r="D6" s="10">
-        <f>B6+C6</f>
+      <c r="D7" s="10">
+        <f t="shared" si="0"/>
         <v>3.1560000000000001</v>
       </c>
-      <c r="E6" s="11">
-        <f t="shared" ref="E6:E12" si="2">(D6-$D$3)/$D$3</f>
+      <c r="E7" s="11">
+        <f t="shared" si="1"/>
         <v>1.8078291814946621</v>
       </c>
-      <c r="F6" s="11">
-        <f t="shared" si="1"/>
+      <c r="F7" s="11">
+        <f t="shared" si="2"/>
         <v>0.54705882352941182</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G7" s="12" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B8" s="13">
         <v>6.524</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C8" s="13">
         <v>0.184</v>
       </c>
-      <c r="D7" s="16">
-        <f>B7+C7</f>
+      <c r="D8" s="13">
+        <f t="shared" si="0"/>
         <v>6.7080000000000002</v>
       </c>
-      <c r="E7" s="17">
-        <f t="shared" ref="E7" si="3">(D7-$D$3)/$D$3</f>
+      <c r="E8" s="14">
+        <f t="shared" si="1"/>
         <v>4.9679715302491116</v>
       </c>
-      <c r="F7" s="17">
-        <f>(D7-D5)/D5</f>
-        <v>2.2882352941176469</v>
-      </c>
-      <c r="G7" s="18" t="s">
+      <c r="F8" s="14">
+        <f t="shared" si="2"/>
+        <v>1.1254752851711027</v>
+      </c>
+      <c r="G8" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B9" s="3">
         <v>14.616</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C9" s="3">
         <v>0.90800000000000003</v>
       </c>
-      <c r="D8" s="3">
-        <f>B8+C8</f>
+      <c r="D9" s="13">
+        <f t="shared" si="0"/>
         <v>15.523999999999999</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E9" s="14">
+        <f t="shared" si="1"/>
+        <v>12.811387900355871</v>
+      </c>
+      <c r="F9" s="14">
         <f t="shared" si="2"/>
-        <v>12.811387900355871</v>
-      </c>
-      <c r="F8" s="4">
-        <f>(D8-D6)/D6</f>
-        <v>3.9188846641318116</v>
-      </c>
-      <c r="G8" s="5" t="s">
+        <v>1.3142516398330351</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B10" s="3">
         <v>18.655999999999999</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C10" s="3">
         <v>0.34799999999999998</v>
       </c>
-      <c r="D9" s="3">
-        <f>B9+C9</f>
+      <c r="D10" s="13">
+        <f t="shared" si="0"/>
         <v>19.003999999999998</v>
       </c>
-      <c r="E9" s="4">
-        <f>(D9-$D$3)/$D$3</f>
+      <c r="E10" s="14">
+        <f t="shared" si="1"/>
         <v>15.907473309608541</v>
       </c>
-      <c r="F9" s="4">
-        <f>(D9-D8)/D8</f>
+      <c r="F10" s="14">
+        <f t="shared" si="2"/>
         <v>0.22416902860087598</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G10" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B11" s="3">
         <v>20.776</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C11" s="3">
         <v>0.33600000000000002</v>
       </c>
-      <c r="D10" s="3">
-        <f>B10+C10</f>
+      <c r="D11" s="13">
+        <f t="shared" si="0"/>
         <v>21.111999999999998</v>
       </c>
-      <c r="E10" s="4">
-        <f>(D10-$D$3)/$D$3</f>
+      <c r="E11" s="14">
+        <f t="shared" si="1"/>
         <v>17.782918149466195</v>
       </c>
-      <c r="F10" s="4">
-        <f>(D10-D9)/D9</f>
+      <c r="F11" s="14">
+        <f t="shared" si="2"/>
         <v>0.11092401599663233</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G11" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B12" s="3">
         <v>25.044</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C12" s="3">
         <v>0.23599999999999999</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D12" s="13">
         <f t="shared" si="0"/>
         <v>25.28</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E12" s="14">
+        <f t="shared" si="1"/>
+        <v>21.491103202846979</v>
+      </c>
+      <c r="F12" s="14">
         <f t="shared" si="2"/>
-        <v>21.491103202846979</v>
-      </c>
-      <c r="F11" s="4">
-        <f>(D11-D10)/D10</f>
         <v>0.19742326638878377</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G12" s="6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B13" s="3">
         <v>66.444000000000003</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C13" s="3">
         <v>2.34</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D13" s="13">
         <f t="shared" si="0"/>
         <v>68.784000000000006</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E13" s="14">
+        <f t="shared" si="1"/>
+        <v>60.19572953736656</v>
+      </c>
+      <c r="F13" s="14">
         <f t="shared" si="2"/>
-        <v>60.19572953736656</v>
-      </c>
-      <c r="F12" s="4">
-        <f t="shared" si="1"/>
         <v>1.7208860759493672</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G13" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="21" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
         <v>54</v>
       </c>
     </row>
@@ -934,7 +966,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -943,24 +975,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13" t="s">
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="15" t="s">
+      <c r="F1" s="22"/>
+      <c r="G1" s="23" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
+      <c r="A2" s="21"/>
       <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
@@ -976,7 +1008,7 @@
       <c r="F2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="21"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1220,7 +1252,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="18" t="s">
         <v>53</v>
       </c>
       <c r="B13" s="3"/>
@@ -1254,24 +1286,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13" t="s">
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="15" t="s">
+      <c r="F1" s="22"/>
+      <c r="G1" s="23" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
+      <c r="A2" s="21"/>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1287,7 +1319,7 @@
       <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="21"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1439,7 +1471,7 @@
         <f t="shared" si="1"/>
         <v>0.54447377481923531</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="20" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1522,7 +1554,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="18" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>